<commit_message>
Added title to the graphs axes
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15CB118-80F6-4356-B2D9-54DC19A37D98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328884B-E35A-4309-99D7-F31DC48A7B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,6 +534,60 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> #</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -596,6 +650,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1260,6 +1368,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1322,6 +1479,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1953,6 +2159,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2015,6 +2270,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2670,6 +2974,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2732,6 +3085,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3461,6 +3863,60 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> #</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3523,6 +3979,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4123,6 +4628,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4185,6 +4739,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4809,6 +5412,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4871,6 +5523,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5471,6 +6172,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5533,6 +6283,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6157,6 +6956,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6219,6 +7067,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6545,6 +7442,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6607,6 +7553,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6895,6 +7890,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6957,6 +8001,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7616,6 +8709,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7678,6 +8820,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7978,6 +9169,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8040,6 +9280,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Percentage Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8626,6 +9915,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8688,6 +10026,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9290,6 +10677,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9352,6 +10788,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9979,6 +11464,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10041,6 +11575,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10692,6 +12275,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10754,6 +12386,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11359,6 +13040,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11421,6 +13151,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -12050,6 +13829,55 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test #</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -12112,6 +13940,55 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -22828,8 +24705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U29"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23212,8 +25089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C216289-8C12-498E-A0E3-71650F3444CE}">
   <dimension ref="C7:P9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23342,8 +25219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306EBCAD-CACF-4C45-B6AB-C5660DFC9901}">
   <dimension ref="C4:V8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23638,8 +25515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38478DB4-3557-4910-B8FA-B2B513BB4430}">
   <dimension ref="C3:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23908,8 +25785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E897947A-A8E4-4A23-8CE5-CEE211D032C2}">
   <dimension ref="C4:V12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24208,8 +26085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8F5EA9-4FF5-47A7-AB2D-15BEFA17A709}">
   <dimension ref="B3:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24460,7 +26337,7 @@
   <dimension ref="B4:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F9"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24710,8 +26587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CEBFAB-1780-48D4-BCA6-3DC69FA75354}">
   <dimension ref="C5:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
removed not used graph, fixed a title
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328884B-E35A-4309-99D7-F31DC48A7B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FEE305-FD2D-4C13-A59B-1A2BBB026428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3271,900 +3271,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Harmless Initial Transactions</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Variation</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Simulation 1</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:extLst>
-                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:fullRef>
-                      <c15:sqref>'Set 7'!$J$6:$O$6</c15:sqref>
-                    </c15:fullRef>
-                  </c:ext>
-                </c:extLst>
-                <c:f>'Set 7'!$K$6:$O$6</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>1.632666E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.5993719999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1.7118910000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.6614859999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.450502E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:extLst>
-                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:fullRef>
-                      <c15:sqref>'Set 7'!$J$6:$O$6</c15:sqref>
-                    </c15:fullRef>
-                  </c:ext>
-                </c:extLst>
-                <c:f>'Set 7'!$K$6:$O$6</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>1.632666E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.5993719999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1.7118910000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.6614859999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.450502E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx2">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="5"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Set 7'!$J$4:$O$4</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Set 7'!$K$4:$O$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.56645909999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.57054859999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.57361030000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.56567979999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.566492</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F009-4353-A76F-DBD6DB12955E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Simulation 2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:extLst>
-                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:fullRef>
-                      <c15:sqref>'Set 7'!$Q$6:$V$6</c15:sqref>
-                    </c15:fullRef>
-                  </c:ext>
-                </c:extLst>
-                <c:f>'Set 7'!$R$6:$V$6</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>3.8760629999999997E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.6299259999999997E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.9143260000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.1817290000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.1200572</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:extLst>
-                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                    <c15:fullRef>
-                      <c15:sqref>'Set 7'!$Q$6:$V$6</c15:sqref>
-                    </c15:fullRef>
-                  </c:ext>
-                </c:extLst>
-                <c:f>'Set 7'!$R$6:$V$6</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>3.8760629999999997E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.6299259999999997E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.9143260000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.1817290000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.1200572</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="tx2">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="5"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Set 7'!$Q$4:$V$4</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Set 7'!$R$4:$V$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2.725549</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.6356850000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4702259999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.419724</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1759149999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F009-4353-A76F-DBD6DB12955E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="100"/>
-        <c:overlap val="-24"/>
-        <c:axId val="209251535"/>
-        <c:axId val="1918641839"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>Simulation 0</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:gradFill rotWithShape="1">
-                    <a:gsLst>
-                      <a:gs pos="0">
-                        <a:schemeClr val="accent2">
-                          <a:satMod val="103000"/>
-                          <a:lumMod val="102000"/>
-                          <a:tint val="94000"/>
-                        </a:schemeClr>
-                      </a:gs>
-                      <a:gs pos="50000">
-                        <a:schemeClr val="accent2">
-                          <a:satMod val="110000"/>
-                          <a:lumMod val="100000"/>
-                          <a:shade val="100000"/>
-                        </a:schemeClr>
-                      </a:gs>
-                      <a:gs pos="100000">
-                        <a:schemeClr val="accent2">
-                          <a:lumMod val="99000"/>
-                          <a:satMod val="120000"/>
-                          <a:shade val="78000"/>
-                        </a:schemeClr>
-                      </a:gs>
-                    </a:gsLst>
-                    <a:lin ang="5400000" scaled="0"/>
-                  </a:gradFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:errBars>
-                  <c:errBarType val="both"/>
-                  <c:errValType val="cust"/>
-                  <c:noEndCap val="0"/>
-                  <c:plus>
-                    <c:numRef>
-                      <c:extLst>
-                        <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                          <c15:fullRef>
-                            <c15:sqref>'Set 7'!$C$6:$H$6</c15:sqref>
-                          </c15:fullRef>
-                          <c15:formulaRef>
-                            <c15:sqref>'Set 7'!$D$6:$H$6</c15:sqref>
-                          </c15:formulaRef>
-                        </c:ext>
-                      </c:extLst>
-                      <c:numCache>
-                        <c:formatCode>General</c:formatCode>
-                        <c:ptCount val="5"/>
-                        <c:pt idx="0">
-                          <c:v>18.02319</c:v>
-                        </c:pt>
-                        <c:pt idx="1">
-                          <c:v>15.939109999999999</c:v>
-                        </c:pt>
-                        <c:pt idx="2">
-                          <c:v>16.09206</c:v>
-                        </c:pt>
-                        <c:pt idx="3">
-                          <c:v>18.119160000000001</c:v>
-                        </c:pt>
-                        <c:pt idx="4">
-                          <c:v>16.89471</c:v>
-                        </c:pt>
-                      </c:numCache>
-                    </c:numRef>
-                  </c:plus>
-                  <c:minus>
-                    <c:numRef>
-                      <c:extLst>
-                        <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                          <c15:fullRef>
-                            <c15:sqref>'Set 7'!$C$6:$H$6</c15:sqref>
-                          </c15:fullRef>
-                          <c15:formulaRef>
-                            <c15:sqref>'Set 7'!$D$6:$H$6</c15:sqref>
-                          </c15:formulaRef>
-                        </c:ext>
-                      </c:extLst>
-                      <c:numCache>
-                        <c:formatCode>General</c:formatCode>
-                        <c:ptCount val="5"/>
-                        <c:pt idx="0">
-                          <c:v>18.02319</c:v>
-                        </c:pt>
-                        <c:pt idx="1">
-                          <c:v>15.939109999999999</c:v>
-                        </c:pt>
-                        <c:pt idx="2">
-                          <c:v>16.09206</c:v>
-                        </c:pt>
-                        <c:pt idx="3">
-                          <c:v>18.119160000000001</c:v>
-                        </c:pt>
-                        <c:pt idx="4">
-                          <c:v>16.89471</c:v>
-                        </c:pt>
-                      </c:numCache>
-                    </c:numRef>
-                  </c:minus>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:errBars>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>'Set 7'!$C$4:$H$4</c15:sqref>
-                        </c15:fullRef>
-                        <c15:formulaRef>
-                          <c15:sqref>'Set 7'!$D$4:$H$4</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="5"/>
-                      <c:pt idx="0">
-                        <c:v>107.69589999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>103.89</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>100.7931</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>132.14269999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>123.17959999999999</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-F009-4353-A76F-DBD6DB12955E}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="209251535"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx2"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Test</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> #</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1918641839"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1918641839"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx2"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Detection Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="209251535"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx2"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
               <a:t>Interaction Frequency Variation</a:t>
             </a:r>
           </a:p>
@@ -4893,7 +3999,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5677,7 +4783,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6437,7 +5543,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7221,7 +6327,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7707,7 +6813,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8019,7 +7125,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Detection Time (s)</a:t>
+                  <a:t>Percentage Ratio</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -14391,43 +13497,6 @@
 </file>
 
 <file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -14464,7 +13533,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -19025,475 +18094,6 @@
 </file>
 
 <file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700">
-        <a:solidFill>
-          <a:schemeClr val="lt2"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="302">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -24170,42 +22770,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB4F1EB-7208-492B-9280-B7DBD08C6BB2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -24705,8 +23269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U29"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView topLeftCell="M7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25515,7 +24079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38478DB4-3557-4910-B8FA-B2B513BB4430}">
   <dimension ref="C3:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
@@ -25785,8 +24349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E897947A-A8E4-4A23-8CE5-CEE211D032C2}">
   <dimension ref="C4:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26085,7 +24649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8F5EA9-4FF5-47A7-AB2D-15BEFA17A709}">
   <dimension ref="B3:R7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -26588,7 +25152,7 @@
   <dimension ref="C5:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added percentuale variation of the resutls
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FEE305-FD2D-4C13-A59B-1A2BBB026428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCC0BD1-FE1A-479B-BD64-BC22331EDF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="1725" windowWidth="21600" windowHeight="11325" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Set 8" sheetId="6" r:id="rId6"/>
     <sheet name="Set 9" sheetId="7" r:id="rId7"/>
     <sheet name="Set 10 (Sim 2)" sheetId="8" r:id="rId8"/>
+    <sheet name="Average percentuale variation" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,16 +39,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Sim0-&gt;Sim1</t>
+  </si>
+  <si>
+    <t>Sim0-&gt;Sim2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,13 +75,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,19 +113,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -22659,16 +22690,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>127635</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>432435</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23267,15 +23298,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U29"/>
+  <dimension ref="B4:Z32"/>
   <sheetViews>
-    <sheetView topLeftCell="M7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z32" activeCellId="1" sqref="Q32 Z32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4.5390360000000003</v>
       </c>
@@ -23331,7 +23362,7 @@
         <v>2.799436</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>7.9502920000000001</v>
       </c>
@@ -23387,7 +23418,7 @@
         <v>0.1792936</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1.5582290000000001</v>
       </c>
@@ -23443,7 +23474,7 @@
         <v>3.5140890000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>22</v>
       </c>
@@ -23499,7 +23530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>78</v>
       </c>
@@ -23555,92 +23586,93 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D27" s="2">
-        <f>(P4-B4)/B4</f>
-        <v>-0.67609906596907365</v>
-      </c>
+    <row r="27" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="D28" s="2">
-        <f>(B4-P4)/P4</f>
-        <v>2.0873637428428014</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" ref="E28:I28" si="0">(C4-Q4)/Q4</f>
-        <v>5.5755633417516046</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="0"/>
-        <v>5.3757346687716661</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>14.085554770711473</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>44.23286868076854</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="0"/>
-        <v>66.936327174473718</v>
-      </c>
+    <row r="28" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="O28" s="2">
-        <f>(I4-P4)/P4</f>
-        <v>-0.72685087314769847</v>
-      </c>
-      <c r="P28" s="2">
-        <f t="shared" ref="P28:T28" si="1">(J4-Q4)/Q4</f>
-        <v>-0.72270086220417218</v>
-      </c>
-      <c r="Q28" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.7639076273137837</v>
-      </c>
-      <c r="R28" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.78639622602117687</v>
-      </c>
-      <c r="S28" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.79511639673328205</v>
-      </c>
-      <c r="T28" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.78946559235503166</v>
-      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.3">
-      <c r="O29" s="2">
-        <f>(P4-I4)/I4</f>
-        <v>2.661003831583634</v>
-      </c>
-      <c r="P29" s="2">
-        <f t="shared" ref="P29:T29" si="2">(Q4-J4)/J4</f>
-        <v>2.6062138813294413</v>
-      </c>
-      <c r="Q29" s="2">
-        <f t="shared" si="2"/>
-        <v>3.23563026887392</v>
-      </c>
-      <c r="R29" s="2">
-        <f t="shared" si="2"/>
-        <v>3.6815652241197805</v>
-      </c>
-      <c r="S29" s="2">
-        <f t="shared" si="2"/>
-        <v>3.8808200561476727</v>
-      </c>
-      <c r="T29" s="2">
-        <f t="shared" si="2"/>
-        <v>3.749817434527543</v>
+    <row r="29" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+    </row>
+    <row r="32" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <f>(B4-I4)/B4</f>
+        <v>0.91152674268280764</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ref="L32:P32" si="0">(C4-J4)/C4</f>
+        <v>0.95782883938854113</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>0.96297016972136629</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0.98584050920066046</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>0.99547047071648975</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>0.9969010039782652</v>
+      </c>
+      <c r="Q32" s="4">
+        <f>AVERAGE(K32:P32)</f>
+        <v>0.96842295594802164</v>
+      </c>
+      <c r="T32">
+        <f>(B4-P4)/B4</f>
+        <v>0.67609906596907365</v>
+      </c>
+      <c r="U32">
+        <f t="shared" ref="U32:Y32" si="1">(C4-Q4)/C4</f>
+        <v>0.84792177521118384</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="1"/>
+        <v>0.84315533002055465</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="1"/>
+        <v>0.93371142028256759</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="1"/>
+        <v>0.9778921826281346</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="1"/>
+        <v>0.98528033466643239</v>
+      </c>
+      <c r="Z32" s="4">
+        <f>AVERAGE(T32:Y32)</f>
+        <v>0.87734335146299125</v>
       </c>
     </row>
   </sheetData>
@@ -23651,15 +23683,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C216289-8C12-498E-A0E3-71650F3444CE}">
-  <dimension ref="C7:P9"/>
+  <dimension ref="C7:P30"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="P30" activeCellId="1" sqref="J30 P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>123.28440000000001</v>
       </c>
@@ -23697,7 +23729,7 @@
         <v>2.681683</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>89.575879999999998</v>
       </c>
@@ -23735,7 +23767,7 @@
         <v>0.27015139999999999</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>17.556550000000001</v>
       </c>
@@ -23771,6 +23803,48 @@
       </c>
       <c r="P9">
         <v>5.2948710000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f>(C7-H7)/C7</f>
+        <v>0.99547047071648975</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:I30" si="0">(D7-I7)/D7</f>
+        <v>0.99549890752627657</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>0.99546371771632036</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0.99555695778520559</v>
+      </c>
+      <c r="J30" s="4">
+        <f>AVERAGE(F30:I30)</f>
+        <v>0.99549751343607307</v>
+      </c>
+      <c r="L30">
+        <f>(C7-M7)/C7</f>
+        <v>0.9778921826281346</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ref="M30:O30" si="1">(D7-N7)/D7</f>
+        <v>0.97953026428030643</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>0.97834538569162122</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>0.97871374379970455</v>
+      </c>
+      <c r="P30" s="4">
+        <f>AVERAGE(L30:O30)</f>
+        <v>0.97862039409994173</v>
       </c>
     </row>
   </sheetData>
@@ -23781,15 +23855,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306EBCAD-CACF-4C45-B6AB-C5660DFC9901}">
-  <dimension ref="C4:V8"/>
+  <dimension ref="C4:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W30" activeCellId="1" sqref="N30 W30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>662.98609999999996</v>
       </c>
@@ -23845,7 +23919,7 @@
         <v>2.648355</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>441.16059999999999</v>
       </c>
@@ -23901,7 +23975,7 @@
         <v>0.21315029999999999</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>86.465900000000005</v>
       </c>
@@ -23957,7 +24031,7 @@
         <v>4.1776679999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -24013,7 +24087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>99</v>
       </c>
@@ -24067,6 +24141,64 @@
       </c>
       <c r="V8">
         <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f>(C4-J4)/C4</f>
+        <v>0.96150198322408276</v>
+      </c>
+      <c r="I30">
+        <f t="shared" ref="I30:M30" si="0">(D4-K4)/D4</f>
+        <v>0.95272145230274885</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0.99418969662526524</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>0.99580467388443905</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0.99490842701810289</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>0.99479839795138791</v>
+      </c>
+      <c r="N30" s="4">
+        <f>AVERAGE(H30:M30)</f>
+        <v>0.98232077183433775</v>
+      </c>
+      <c r="Q30">
+        <f>(C4-Q4)/C4</f>
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <f t="shared" ref="R30:V30" si="1">(D4-R4)/D4</f>
+        <v>0.88413070084420298</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="1"/>
+        <v>0.9743254044345725</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="1"/>
+        <v>0.9799248249609892</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="1"/>
+        <v>0.97589708629366345</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="1"/>
+        <v>0.97553457818047118</v>
+      </c>
+      <c r="W30" s="4">
+        <f>AVERAGE(R30:V30)</f>
+        <v>0.95796251894277984</v>
       </c>
     </row>
   </sheetData>
@@ -24077,15 +24209,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38478DB4-3557-4910-B8FA-B2B513BB4430}">
-  <dimension ref="C3:S28"/>
+  <dimension ref="C3:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S29" activeCellId="1" sqref="K29 S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>116.2533</v>
       </c>
@@ -24132,7 +24264,7 @@
         <v>162.68870000000001</v>
       </c>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>78.95147</v>
       </c>
@@ -24179,7 +24311,7 @@
         <v>98.61591</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>15.4742</v>
       </c>
@@ -24226,7 +24358,7 @@
         <v>19.32836</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -24273,7 +24405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>99</v>
       </c>
@@ -24320,23 +24452,59 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="R14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G28">
-        <f>16145.53/422</f>
-        <v>38.259549763033178</v>
-      </c>
-      <c r="H28">
-        <f>M3/L3</f>
-        <v>9.7347568832464884</v>
-      </c>
-      <c r="I28">
-        <f>S3/R3</f>
-        <v>7.3412596166125255</v>
+    <row r="29" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f>(C3-I3)/C3</f>
+        <v>0.99986668215009811</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:J29" si="0">(D3-J3)/D3</f>
+        <v>0.99936259558209262</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0.99547047071648975</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.98674173582582547</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0.99662389032753962</v>
+      </c>
+      <c r="K29" s="4">
+        <f>AVERAGE(F29:J29)</f>
+        <v>0.99561307492040907</v>
+      </c>
+      <c r="N29">
+        <f>(C3-O3)/C3</f>
+        <v>0.99712565664802633</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:R29" si="1">(D3-P3)/D3</f>
+        <v>0.99463826550543022</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.9778921826281346</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.9475277445629654</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.9899236073389972</v>
+      </c>
+      <c r="S29" s="4">
+        <f>AVERAGE(N29:R29)</f>
+        <v>0.98142149133671075</v>
       </c>
     </row>
   </sheetData>
@@ -24347,15 +24515,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E897947A-A8E4-4A23-8CE5-CEE211D032C2}">
-  <dimension ref="C4:V12"/>
+  <dimension ref="C4:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>123.28440000000001</v>
       </c>
@@ -24411,7 +24579,7 @@
         <v>2.1759149999999998</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>89.575879999999998</v>
       </c>
@@ -24467,7 +24635,7 @@
         <v>0.61254810000000004</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>17.556550000000001</v>
       </c>
@@ -24523,7 +24691,7 @@
         <v>0.1200572</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -24579,7 +24747,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>97</v>
       </c>
@@ -24635,8 +24803,66 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="O12" s="3"/>
+    </row>
+    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>(C4-J4)/C4</f>
+        <v>0.99547047071648975</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:J29" si="0">(D4-K4)/D4</f>
+        <v>0.99474019809482062</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>0.99450814707864088</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0.9943090320666792</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.99571917480118088</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0.99540108914138381</v>
+      </c>
+      <c r="K29" s="4">
+        <f>AVERAGE(E29:J29)</f>
+        <v>0.99502468531653265</v>
+      </c>
+      <c r="N29">
+        <f>(C4-Q4)/C4</f>
+        <v>0.9277894283461654</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:S29" si="1">(D4-R4)/D4</f>
+        <v>0.97469217491102256</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.9746300413899317</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.97549211205925801</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.98168855335936078</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="1"/>
+        <v>0.9823354272947793</v>
+      </c>
+      <c r="T29" s="4">
+        <f>AVERAGE(N29:S29)</f>
+        <v>0.96943795622675299</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24647,15 +24873,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8F5EA9-4FF5-47A7-AB2D-15BEFA17A709}">
-  <dimension ref="B3:R7"/>
+  <dimension ref="B3:R29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R29" activeCellId="1" sqref="J29 R29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>100.7766</v>
       </c>
@@ -24702,7 +24928,7 @@
         <v>2.7073589999999998</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>86.271680000000003</v>
       </c>
@@ -24749,7 +24975,7 @@
         <v>0.24123159999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>16.908940000000001</v>
       </c>
@@ -24796,7 +25022,7 @@
         <v>4.7280530000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -24843,7 +25069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>96</v>
       </c>
@@ -24888,6 +25114,56 @@
       </c>
       <c r="R7">
         <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>(B3-H3)/B3</f>
+        <v>0.99431821375200202</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:I29" si="0">(C3-I3)/C3</f>
+        <v>0.98628375898129728</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>0.99707157966450177</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0.99976864347927508</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.99997475813701686</v>
+      </c>
+      <c r="J29" s="4">
+        <f>AVERAGE(E29:I29)</f>
+        <v>0.99548339080281867</v>
+      </c>
+      <c r="M29">
+        <f>(B3-N3)/B3</f>
+        <v>0.98137568641926787</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:Q29" si="1">(C3-O3)/C3</f>
+        <v>0.93820381712013656</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0.98629391103967168</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.99889434571323599</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.99987866700189032</v>
+      </c>
+      <c r="R29" s="4">
+        <f>AVERAGE(M29:Q29)</f>
+        <v>0.98092928545884051</v>
       </c>
     </row>
   </sheetData>
@@ -24898,15 +25174,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBEEE35-85AF-42CA-8BFA-768200CAE9AB}">
-  <dimension ref="B4:R8"/>
+  <dimension ref="B4:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="S29" activeCellId="1" sqref="L29 S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>21.639559999999999</v>
       </c>
@@ -24953,7 +25229,7 @@
         <v>35.218170000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>40.38944</v>
       </c>
@@ -25000,7 +25276,7 @@
         <v>17.211839999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>7.9161849999999996</v>
       </c>
@@ -25047,7 +25323,7 @@
         <v>3.3734600000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -25094,7 +25370,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>46</v>
       </c>
@@ -25139,6 +25415,56 @@
       </c>
       <c r="R8">
         <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f>(B4-H4)/B4</f>
+        <v>0.98587888108630684</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:K29" si="0">(C4-I4)/C4</f>
+        <v>0.98869411023678233</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0.99542963678035956</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0.99140906018582842</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>0.99556340954833089</v>
+      </c>
+      <c r="L29" s="4">
+        <f>AVERAGE(G29:K29)</f>
+        <v>0.99139501956752163</v>
+      </c>
+      <c r="N29">
+        <f>(B4-N4)/B4</f>
+        <v>0.95885946849196557</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:R29" si="1">(C4-O4)/C4</f>
+        <v>0.95694562859447285</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>0.97510603056271639</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>0.94923834456929845</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.98722845641964785</v>
+      </c>
+      <c r="S29" s="4">
+        <f>AVERAGE(N29:R29)</f>
+        <v>0.96547558572762016</v>
       </c>
     </row>
   </sheetData>
@@ -25151,13 +25477,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CEBFAB-1780-48D4-BCA6-3DC69FA75354}">
   <dimension ref="C5:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2.3639890000000001</v>
       </c>
@@ -25171,7 +25497,7 @@
         <v>2.1133150000000001</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>0.30873420000000001</v>
       </c>
@@ -25185,7 +25511,7 @@
         <v>0.47999570000000003</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>6.0510790000000002E-2</v>
       </c>
@@ -25199,7 +25525,7 @@
         <v>9.4077439999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
@@ -25213,7 +25539,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>97</v>
       </c>
@@ -25231,4 +25557,96 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D7D066-7EAF-4F60-9AB6-0801A04E18F0}">
+  <dimension ref="B3:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>0.96842295594802164</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.87734335146299125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>0.99549751343607307</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.97862039409994173</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>0.98232077183433775</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.95796251894277984</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>0.99561307492040907</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.98142149133671075</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>0.99502468531653265</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.96943795622675299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>0.99548339080281867</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.98092928545884051</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>0.99139501956752163</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.96547558572762016</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <f>AVERAGE(B4:B10)</f>
+        <v>0.98910820168938773</v>
+      </c>
+      <c r="C11" s="5">
+        <f>AVERAGE(C4:C10)</f>
+        <v>0.95874151189366241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added results from simulation on Tribler network
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1217A82C-4DA3-4159-B58F-FC4929EB898D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BF94A9-2B63-4A11-9D32-FD2AA98B4E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Set 9" sheetId="7" r:id="rId7"/>
     <sheet name="Set 10 (Sim 2)" sheetId="8" r:id="rId8"/>
     <sheet name="Average percentuale variation" sheetId="9" r:id="rId9"/>
+    <sheet name="Set 12 - Tribler Network" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -67,12 +68,24 @@
   <si>
     <t>1000000kbps</t>
   </si>
+  <si>
+    <t>Simulation 0</t>
+  </si>
+  <si>
+    <t>Simulation 1</t>
+  </si>
+  <si>
+    <t>Set 12 - Tribler network</t>
+  </si>
+  <si>
+    <t>Simulation 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +121,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -136,7 +157,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -148,6 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -25764,13 +25786,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>4.5390360000000003</v>
       </c>
@@ -25826,7 +25848,7 @@
         <v>2.799436</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>7.9502920000000001</v>
       </c>
@@ -25882,7 +25904,7 @@
         <v>0.1792936</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>1.5582290000000001</v>
       </c>
@@ -25938,7 +25960,7 @@
         <v>3.5140890000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>22</v>
       </c>
@@ -25994,7 +26016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>78</v>
       </c>
@@ -26050,14 +26072,14 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:26" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:26" x14ac:dyDescent="0.3">
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -26073,7 +26095,7 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:26" x14ac:dyDescent="0.3">
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
@@ -26081,7 +26103,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="32" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:26" x14ac:dyDescent="0.3">
       <c r="K32">
         <f>(B4-I4)/B4</f>
         <v>0.91152674268280764</v>
@@ -26142,6 +26164,344 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EED80D-1FFC-4B2F-BCEF-819117E61827}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>77.552748834100996</v>
+      </c>
+      <c r="C2">
+        <v>0.408255574249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>132.59328535419201</v>
+      </c>
+      <c r="C3">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>0.61000000000200005</v>
+      </c>
+      <c r="C4">
+        <v>0.40736063949700002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>106.117938129187</v>
+      </c>
+      <c r="C5">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C6">
+        <v>0.40781291242099998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C7">
+        <v>0.406666666668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>231.46499484135401</v>
+      </c>
+      <c r="C8">
+        <v>0.40666666667000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>37.768497183866998</v>
+      </c>
+      <c r="C9">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C10">
+        <v>0.40728345526900001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>159.24149484771701</v>
+      </c>
+      <c r="C11">
+        <v>0.406666666668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>59.959975171487997</v>
+      </c>
+      <c r="C12">
+        <v>0.50878415680300004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>65.911153211772998</v>
+      </c>
+      <c r="C13">
+        <v>0.40767251090500001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>187.42766439342</v>
+      </c>
+      <c r="C14">
+        <v>0.41018216037999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>96.496597888729994</v>
+      </c>
+      <c r="C15">
+        <v>0.50922963020400003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0.50833333333499997</v>
+      </c>
+      <c r="C16">
+        <v>0.50845557031599997</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>93.088975306747002</v>
+      </c>
+      <c r="C17">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>25.644209351699999</v>
+      </c>
+      <c r="C18">
+        <v>0.406666666668</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>146.686686150822</v>
+      </c>
+      <c r="C19">
+        <v>0.40666666667000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>126.28601949976699</v>
+      </c>
+      <c r="C20">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>6.8681103691379999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>206.180580524639</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>108.935763302745</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>0.61000000000200005</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>57.004984865182003</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0.406666666668</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>81.924129276520006</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>172.58504778538099</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>112.22294146845501</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>82.493223301520004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>66.505326795643001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>69.807717030917999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>247.577805762926</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>244.51641065726699</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>219.029127908878</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>148.981853841163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>0.50833333333499997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>14.368073256500001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0.61000000000200005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>249.06878495392399</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>86.681269999999998</v>
+      </c>
+      <c r="C45">
+        <v>0.45000190000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>81.924459999999996</v>
+      </c>
+      <c r="C46">
+        <v>5.1275830000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>16.056899999999999</v>
+      </c>
+      <c r="C47">
+        <v>1.0049880000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>42</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -26153,9 +26513,9 @@
       <selection activeCell="P30" activeCellId="1" sqref="J30 P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>123.28440000000001</v>
       </c>
@@ -26193,7 +26553,7 @@
         <v>2.681683</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>89.575879999999998</v>
       </c>
@@ -26231,7 +26591,7 @@
         <v>0.27015139999999999</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>17.556550000000001</v>
       </c>
@@ -26269,7 +26629,7 @@
         <v>5.2948710000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:16" x14ac:dyDescent="0.3">
       <c r="F30">
         <f>(C7-H7)/C7</f>
         <v>0.99547047071648975</v>
@@ -26325,9 +26685,9 @@
       <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>662.98609999999996</v>
       </c>
@@ -26383,7 +26743,7 @@
         <v>2.648355</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>441.16059999999999</v>
       </c>
@@ -26439,7 +26799,7 @@
         <v>0.21315029999999999</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>86.465900000000005</v>
       </c>
@@ -26495,7 +26855,7 @@
         <v>4.1776679999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>1</v>
       </c>
@@ -26551,7 +26911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>99</v>
       </c>
@@ -26607,7 +26967,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H30">
         <f>(C4-J4)/C4</f>
         <v>0.96150198322408276</v>
@@ -26665,32 +27025,32 @@
         <v>0.95796251894277984</v>
       </c>
     </row>
-    <row r="40" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P40" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P41" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P42" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P43" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P44" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P45" s="6" t="s">
         <v>8</v>
       </c>
@@ -26709,9 +27069,9 @@
       <selection activeCell="S29" activeCellId="1" sqref="K29 S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>116.2533</v>
       </c>
@@ -26758,7 +27118,7 @@
         <v>162.68870000000001</v>
       </c>
     </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>78.95147</v>
       </c>
@@ -26805,7 +27165,7 @@
         <v>98.61591</v>
       </c>
     </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>15.4742</v>
       </c>
@@ -26852,7 +27212,7 @@
         <v>19.32836</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1</v>
       </c>
@@ -26899,7 +27259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>99</v>
       </c>
@@ -26946,12 +27306,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
       <c r="R14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="6:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:19" x14ac:dyDescent="0.3">
       <c r="F29">
         <f>(C3-I3)/C3</f>
         <v>0.99986668215009811</v>
@@ -27015,9 +27375,9 @@
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>123.28440000000001</v>
       </c>
@@ -27073,7 +27433,7 @@
         <v>2.1759149999999998</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>89.575879999999998</v>
       </c>
@@ -27129,7 +27489,7 @@
         <v>0.61254810000000004</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>17.556550000000001</v>
       </c>
@@ -27185,7 +27545,7 @@
         <v>0.1200572</v>
       </c>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3</v>
       </c>
@@ -27241,7 +27601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>97</v>
       </c>
@@ -27297,10 +27657,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
       <c r="O12" s="3"/>
     </row>
-    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:20" x14ac:dyDescent="0.3">
       <c r="E29">
         <f>(C4-J4)/C4</f>
         <v>0.99547047071648975</v>
@@ -27373,9 +27733,9 @@
       <selection activeCell="R29" activeCellId="1" sqref="J29 R29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>100.7766</v>
       </c>
@@ -27422,7 +27782,7 @@
         <v>2.7073589999999998</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>86.271680000000003</v>
       </c>
@@ -27469,7 +27829,7 @@
         <v>0.24123159999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>16.908940000000001</v>
       </c>
@@ -27516,7 +27876,7 @@
         <v>4.7280530000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -27563,7 +27923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>96</v>
       </c>
@@ -27610,7 +27970,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E29">
         <f>(B3-H3)/B3</f>
         <v>0.99431821375200202</v>
@@ -27674,9 +28034,9 @@
       <selection activeCell="S29" activeCellId="1" sqref="L29 S29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>21.639559999999999</v>
       </c>
@@ -27723,7 +28083,7 @@
         <v>35.218170000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>40.38944</v>
       </c>
@@ -27770,7 +28130,7 @@
         <v>17.211839999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>7.9161849999999996</v>
       </c>
@@ -27817,7 +28177,7 @@
         <v>3.3734600000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -27864,7 +28224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>46</v>
       </c>
@@ -27911,7 +28271,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:19" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>(B4-H4)/B4</f>
         <v>0.98587888108630684</v>
@@ -27975,9 +28335,9 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2.3639890000000001</v>
       </c>
@@ -27991,7 +28351,7 @@
         <v>2.1133150000000001</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0.30873420000000001</v>
       </c>
@@ -28005,7 +28365,7 @@
         <v>0.47999570000000003</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>6.0510790000000002E-2</v>
       </c>
@@ -28019,7 +28379,7 @@
         <v>9.4077439999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>3</v>
       </c>
@@ -28033,7 +28393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>97</v>
       </c>
@@ -28061,12 +28421,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -28074,7 +28434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>0.96842295594802164</v>
       </c>
@@ -28082,7 +28442,7 @@
         <v>0.87734335146299125</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>0.99549751343607307</v>
       </c>
@@ -28090,7 +28450,7 @@
         <v>0.97862039409994173</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>0.98232077183433775</v>
       </c>
@@ -28098,7 +28458,7 @@
         <v>0.95796251894277984</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>0.99561307492040907</v>
       </c>
@@ -28106,7 +28466,7 @@
         <v>0.98142149133671075</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>0.99502468531653265</v>
       </c>
@@ -28114,7 +28474,7 @@
         <v>0.96943795622675299</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>0.99548339080281867</v>
       </c>
@@ -28122,7 +28482,7 @@
         <v>0.98092928545884051</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>0.99139501956752163</v>
       </c>
@@ -28130,7 +28490,7 @@
         <v>0.96547558572762016</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <f>AVERAGE(B4:B10)</f>
         <v>0.98910820168938773</v>

</xml_diff>

<commit_message>
Analized data and creatad graphs for set 11
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BF94A9-2B63-4A11-9D32-FD2AA98B4E55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323EA98F-6A7A-4ED8-8ECE-F127257E0E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Set 8" sheetId="6" r:id="rId6"/>
     <sheet name="Set 9" sheetId="7" r:id="rId7"/>
     <sheet name="Set 10 (Sim 2)" sheetId="8" r:id="rId8"/>
-    <sheet name="Average percentuale variation" sheetId="9" r:id="rId9"/>
-    <sheet name="Set 12 - Tribler Network" sheetId="10" r:id="rId10"/>
+    <sheet name="Set 11 (Sim 2)" sheetId="11" r:id="rId9"/>
+    <sheet name="Average percentuale variation" sheetId="9" r:id="rId10"/>
+    <sheet name="Set 12 - Tribler Network" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -80,11 +81,23 @@
   <si>
     <t>Simulation 2</t>
   </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>STD. DEV.</t>
+  </si>
+  <si>
+    <t>Margin Of Error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +170,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -170,6 +183,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -9673,6 +9688,1782 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Evil Anonymizers Report Benign Nodes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>5% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$C$10:$F$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.9310479999999994E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.0064499999999996E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$C$10:$F$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.9310479999999994E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.0064499999999996E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>30% Replies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>50% Replies</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>80% Replies</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>100% Replies</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Set 11 (Sim 2)'!$C$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7499999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77377039999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>30% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$G$10:$J$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3487110000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.3644010000000004E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.0770610000000001E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$G$10:$J$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3487110000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.3644010000000004E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.0770610000000001E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>30% Replies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>50% Replies</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>80% Replies</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>100% Replies</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Set 11 (Sim 2)'!$G$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4933329999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98759619999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>50% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$K$10:$N$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.8548960000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6988109999999996E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.8686260000000003E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.6444360000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$K$10:$N$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.8548960000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6988109999999996E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.8686260000000003E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.6444360000000001E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>30% Replies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>50% Replies</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>80% Replies</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>100% Replies</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Set 11 (Sim 2)'!$K$8:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.7785709999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41789520000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98683529999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98773529999999987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>80% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$O$10:$R$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.5074110000000003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7941800000000006E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.010197E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.010197E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Set 11 (Sim 2)'!$O$10:$R$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>5.5074110000000003E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7941800000000006E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.010197E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.010197E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>30% Replies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>50% Replies</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>80% Replies</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>100% Replies</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Set 11 (Sim 2)'!$O$8:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.85878420000000011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98725879999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98752780000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98752780000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="698962048"/>
+        <c:axId val="702141440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="698962048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="702141440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="702141440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698962048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Evil Anonymizers Report Benign Nodes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>5% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$C$10:$F$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$C$10:$E$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.9310479999999994E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$C$10:$F$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$C$10:$E$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.9310479999999994E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="3">
+                        <c:v>100% Replies</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c16:filteredLitCache>
+                </c:ext>
+              </c:extLst>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30% Replies</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50% Replies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80% Replies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Set 11 (Sim 2)'!$C$8:$F$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Set 11 (Sim 2)'!$C$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7499999999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>30% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$G$10:$J$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$G$10:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3487110000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.3644010000000004E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$G$10:$J$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$G$10:$I$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.3487110000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.3644010000000004E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="3">
+                        <c:v>100% Replies</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c16:filteredLitCache>
+                </c:ext>
+              </c:extLst>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30% Replies</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50% Replies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80% Replies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Set 11 (Sim 2)'!$G$8:$J$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Set 11 (Sim 2)'!$G$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4933329999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>50% Evilness</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$K$10:$N$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$K$10:$M$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.8548960000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6988109999999996E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.8686260000000003E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 11 (Sim 2)'!$K$10:$N$10</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 11 (Sim 2)'!$K$10:$M$10</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.8548960000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6988109999999996E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.8686260000000003E-5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="3">
+                        <c:v>100% Replies</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c16:filteredLitCache>
+                </c:ext>
+              </c:extLst>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30% Replies</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50% Replies</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80% Replies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Set 11 (Sim 2)'!$K$8:$N$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Set 11 (Sim 2)'!$K$8:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.7785709999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41789520000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98683529999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CFC-4EB6-98E1-0B96899586F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="698962048"/>
+        <c:axId val="702141440"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>80% Evilness</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent4">
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent4">
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:errBars>
+                  <c:errBarType val="both"/>
+                  <c:errValType val="cust"/>
+                  <c:noEndCap val="0"/>
+                  <c:plus>
+                    <c:numRef>
+                      <c:extLst>
+                        <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                          <c15:fullRef>
+                            <c15:sqref>'Set 11 (Sim 2)'!$O$10:$R$10</c15:sqref>
+                          </c15:fullRef>
+                          <c15:formulaRef>
+                            <c15:sqref>'Set 11 (Sim 2)'!$O$10:$Q$10</c15:sqref>
+                          </c15:formulaRef>
+                        </c:ext>
+                      </c:extLst>
+                      <c:numCache>
+                        <c:formatCode>General</c:formatCode>
+                        <c:ptCount val="3"/>
+                        <c:pt idx="0">
+                          <c:v>5.5074110000000003E-4</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>8.7941800000000006E-5</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>1.010197E-4</c:v>
+                        </c:pt>
+                      </c:numCache>
+                    </c:numRef>
+                  </c:plus>
+                  <c:minus>
+                    <c:numRef>
+                      <c:extLst>
+                        <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                          <c15:fullRef>
+                            <c15:sqref>'Set 11 (Sim 2)'!$O$10:$R$10</c15:sqref>
+                          </c15:fullRef>
+                          <c15:formulaRef>
+                            <c15:sqref>'Set 11 (Sim 2)'!$O$10:$Q$10</c15:sqref>
+                          </c15:formulaRef>
+                        </c:ext>
+                      </c:extLst>
+                      <c:numCache>
+                        <c:formatCode>General</c:formatCode>
+                        <c:ptCount val="3"/>
+                        <c:pt idx="0">
+                          <c:v>5.5074110000000003E-4</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>8.7941800000000006E-5</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>1.010197E-4</c:v>
+                        </c:pt>
+                      </c:numCache>
+                    </c:numRef>
+                  </c:minus>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:errBars>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                        <c16:filteredLitCache>
+                          <c:strCache>
+                            <c:ptCount val="1"/>
+                            <c:pt idx="3">
+                              <c:v>100% Replies</c:v>
+                            </c:pt>
+                          </c:strCache>
+                        </c16:filteredLitCache>
+                      </c:ext>
+                    </c:extLst>
+                    <c:f/>
+                    <c:strCache>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>30% Replies</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>50% Replies</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>80% Replies</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>'Set 11 (Sim 2)'!$O$8:$R$8</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>'Set 11 (Sim 2)'!$O$8:$Q$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00%</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>0.85878420000000011</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.98725879999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.98752780000000007</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-4CFC-4EB6-98E1-0B96899586F6}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="698962048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="702141440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="702141440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.0000000000000004E-2"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="698962048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -15114,6 +16905,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors21.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -21243,6 +23114,944 @@
         <a:solidFill>
           <a:schemeClr val="tx2">
             <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -25521,6 +28330,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B69BE9D-A067-4D71-A9BD-88DD5C11971A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2513483-2D4B-4462-B490-4459BD514172}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -26168,10 +29054,104 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D7D066-7EAF-4F60-9AB6-0801A04E18F0}">
+  <dimension ref="B3:C11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>0.96842295594802164</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.87734335146299125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>0.99549751343607307</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.97862039409994173</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>0.98232077183433775</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.95796251894277984</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>0.99561307492040907</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.98142149133671075</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>0.99502468531653265</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.96943795622675299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>0.99548339080281867</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.98092928545884051</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>0.99139501956752163</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.96547558572762016</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <f>AVERAGE(B4:B10)</f>
+        <v>0.98910820168938773</v>
+      </c>
+      <c r="C11" s="5">
+        <f>AVERAGE(C4:C10)</f>
+        <v>0.95874151189366241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EED80D-1FFC-4B2F-BCEF-819117E61827}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28414,93 +31394,308 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D7D066-7EAF-4F60-9AB6-0801A04E18F0}">
-  <dimension ref="B3:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7C7897-AEDC-4797-870C-FDABE33EAE28}">
+  <dimension ref="B3:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5.75</v>
+      </c>
+      <c r="F3">
+        <v>7737.7039999999997</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>54.933329999999998</v>
+      </c>
+      <c r="I3">
+        <v>8296</v>
+      </c>
+      <c r="J3">
+        <v>9875.9619999999995</v>
+      </c>
+      <c r="K3">
+        <v>77.785709999999995</v>
+      </c>
+      <c r="L3">
+        <v>4178.9520000000002</v>
+      </c>
+      <c r="M3">
+        <v>9868.3529999999992</v>
+      </c>
+      <c r="N3">
+        <v>9877.3529999999992</v>
+      </c>
+      <c r="O3">
+        <v>8587.8420000000006</v>
+      </c>
+      <c r="P3">
+        <v>9872.5879999999997</v>
+      </c>
+      <c r="Q3">
+        <v>9875.2780000000002</v>
+      </c>
+      <c r="R3">
+        <v>9875.2780000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="4">
-        <v>0.96842295594802164</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.87734335146299125</v>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2.005674</v>
+      </c>
+      <c r="F4">
+        <v>35.74785</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>6.8813069999999996</v>
+      </c>
+      <c r="I4">
+        <v>27.369890000000002</v>
+      </c>
+      <c r="J4">
+        <v>5.4953130000000003</v>
+      </c>
+      <c r="K4">
+        <v>9.4639279999999992</v>
+      </c>
+      <c r="L4">
+        <v>39.280369999999998</v>
+      </c>
+      <c r="M4">
+        <v>4.0146790000000001</v>
+      </c>
+      <c r="N4">
+        <v>3.3900809999999999</v>
+      </c>
+      <c r="O4">
+        <v>28.099550000000001</v>
+      </c>
+      <c r="P4">
+        <v>4.4869089999999998</v>
+      </c>
+      <c r="Q4">
+        <v>5.1541589999999999</v>
+      </c>
+      <c r="R4">
+        <v>5.1541589999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
-        <v>0.99549751343607307</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.97862039409994173</v>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.39310479999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.0064500000000001</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1.348711</v>
+      </c>
+      <c r="I5">
+        <v>5.364401</v>
+      </c>
+      <c r="J5">
+        <v>1.077061</v>
+      </c>
+      <c r="K5">
+        <v>1.8548960000000001</v>
+      </c>
+      <c r="L5">
+        <v>7.6988110000000001</v>
+      </c>
+      <c r="M5">
+        <v>0.78686259999999997</v>
+      </c>
+      <c r="N5">
+        <v>0.66444360000000002</v>
+      </c>
+      <c r="O5">
+        <v>5.5074110000000003</v>
+      </c>
+      <c r="P5">
+        <v>0.87941800000000003</v>
+      </c>
+      <c r="Q5">
+        <v>1.010197</v>
+      </c>
+      <c r="R5">
+        <v>1.010197</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="4">
-        <v>0.98232077183433775</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.95796251894277984</v>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C8" s="8">
+        <f>C3/10000</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" ref="D8:R8" si="0">D3/10000</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>5.7499999999999999E-4</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.77377039999999997</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>5.4933329999999995E-3</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.8296</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98759619999999992</v>
+      </c>
+      <c r="K8" s="8">
+        <f t="shared" si="0"/>
+        <v>7.7785709999999997E-3</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.41789520000000002</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98683529999999997</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98773529999999987</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.85878420000000011</v>
+      </c>
+      <c r="P8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98725879999999999</v>
+      </c>
+      <c r="Q8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98752780000000007</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98752780000000007</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
-        <v>0.99561307492040907</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.98142149133671075</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
-        <v>0.99502468531653265</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.96943795622675299</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
-        <v>0.99548339080281867</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.98092928545884051</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
-        <v>0.99139501956752163</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.96547558572762016</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
-        <f>AVERAGE(B4:B10)</f>
-        <v>0.98910820168938773</v>
-      </c>
-      <c r="C11" s="5">
-        <f>AVERAGE(C4:C10)</f>
-        <v>0.95874151189366241</v>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C10" s="9">
+        <f t="shared" ref="C9:R10" si="1">C5/10000</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="1"/>
+        <v>3.9310479999999994E-5</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="1"/>
+        <v>7.0064499999999996E-4</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.3487110000000001E-4</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="1"/>
+        <v>5.3644010000000004E-4</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0770610000000001E-4</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.8548960000000001E-4</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" si="1"/>
+        <v>7.6988109999999996E-4</v>
+      </c>
+      <c r="M10" s="9">
+        <f t="shared" si="1"/>
+        <v>7.8686260000000003E-5</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="1"/>
+        <v>6.6444360000000001E-5</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="1"/>
+        <v>5.5074110000000003E-4</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="1"/>
+        <v>8.7941800000000006E-5</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.010197E-4</v>
+      </c>
+      <c r="R10" s="9">
+        <f t="shared" si="1"/>
+        <v>1.010197E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
analized results of evaluation set 12
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DBD23B-B841-4A99-9B0C-FF5000739132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E9C17-C08B-421C-BCDF-1414BA1BF7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Average percentuale variation" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -12429,6 +12430,1044 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Tribler's Network</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Evaluation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AD96-4112-956F-E55166BB067C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-AD96-4112-956F-E55166BB067C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Set 12 - Tribler Network'!$B$56:$D$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>16.056899999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0049880000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.321455E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Set 12 - Tribler Network'!$B$56:$D$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>16.056899999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0049880000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.321455E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>Solution 0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Solution 1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Solution 2</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Set 12 - Tribler Network'!$B$54:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>86.681269999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45000190000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7882979999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD96-4112-956F-E55166BB067C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1051370127"/>
+        <c:axId val="1043781935"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1051370127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Mechanism</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Employed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043781935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1043781935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1051370127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Tribler's</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Network</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Evaluation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-AD96-4112-956F-E55166BB067C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-AD96-4112-956F-E55166BB067C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 12 - Tribler Network'!$B$56:$D$56</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 12 - Tribler Network'!$C$56:$D$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.0049880000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.321455E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:extLst>
+                  <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                    <c15:fullRef>
+                      <c15:sqref>'Set 12 - Tribler Network'!$B$56:$D$56</c15:sqref>
+                    </c15:fullRef>
+                  </c:ext>
+                </c:extLst>
+                <c:f>'Set 12 - Tribler Network'!$C$56:$D$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>1.0049880000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.321455E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Solution 0</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c16:filteredLitCache>
+                </c:ext>
+              </c:extLst>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Solution 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Solution 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Set 12 - Tribler Network'!$B$54:$D$54</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Set 12 - Tribler Network'!$C$54:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.45000190000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7882979999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD96-4112-956F-E55166BB067C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1051370127"/>
+        <c:axId val="1043781935"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1051370127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Mechanism</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Employed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043781935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1043781935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Detection Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1051370127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -18308,6 +19347,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -25604,6 +26717,944 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="302">
   <cs:axisTitle>
@@ -29032,6 +31083,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CB24D62-2860-428E-9A56-5D2063764831}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>522194</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>217394</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4481ECEB-0E75-488C-9B2E-EB169B8B714A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -29995,7 +32123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -30314,11 +32442,11 @@
     </row>
     <row r="32" spans="4:26" x14ac:dyDescent="0.3">
       <c r="K32">
-        <f>(B4-I4)/B4</f>
+        <f t="shared" ref="K32:P32" si="0">(B4-I4)/B4</f>
         <v>0.91152674268280764</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32:P32" si="0">(C4-J4)/C4</f>
+        <f t="shared" si="0"/>
         <v>0.95782883938854113</v>
       </c>
       <c r="M32">
@@ -30342,11 +32470,11 @@
         <v>0.96842295594802164</v>
       </c>
       <c r="T32">
-        <f>(B4-P4)/B4</f>
+        <f t="shared" ref="T32:Y32" si="1">(B4-P4)/B4</f>
         <v>0.67609906596907365</v>
       </c>
       <c r="U32">
-        <f t="shared" ref="U32:Y32" si="1">(C4-Q4)/C4</f>
+        <f t="shared" si="1"/>
         <v>0.84792177521118384</v>
       </c>
       <c r="V32">
@@ -30378,10 +32506,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EED80D-1FFC-4B2F-BCEF-819117E61827}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30411,6 +32539,9 @@
       <c r="C2">
         <v>0.408255574249</v>
       </c>
+      <c r="D2">
+        <v>1.674843791072</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3">
@@ -30419,6 +32550,9 @@
       <c r="C3">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D3">
+        <v>1.6131217457360001</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -30427,6 +32561,9 @@
       <c r="C4">
         <v>0.40736063949700002</v>
       </c>
+      <c r="D4">
+        <v>1.9290386110440001</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
@@ -30435,6 +32572,9 @@
       <c r="C5">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D5">
+        <v>1.8331075058940001</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
@@ -30443,6 +32583,9 @@
       <c r="C6">
         <v>0.40781291242099998</v>
       </c>
+      <c r="D6">
+        <v>1.726893574335</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
@@ -30451,6 +32594,9 @@
       <c r="C7">
         <v>0.406666666668</v>
       </c>
+      <c r="D7">
+        <v>1.53707405849</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
@@ -30459,6 +32605,9 @@
       <c r="C8">
         <v>0.40666666667000001</v>
       </c>
+      <c r="D8">
+        <v>1.8061591923889999</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -30467,6 +32616,9 @@
       <c r="C9">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D9">
+        <v>1.3481723490099999</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
@@ -30475,6 +32627,9 @@
       <c r="C10">
         <v>0.40728345526900001</v>
       </c>
+      <c r="D10">
+        <v>1.7487532856150001</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11">
@@ -30483,6 +32638,9 @@
       <c r="C11">
         <v>0.406666666668</v>
       </c>
+      <c r="D11">
+        <v>1.9171938552800001</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12">
@@ -30491,6 +32649,9 @@
       <c r="C12">
         <v>0.50878415680300004</v>
       </c>
+      <c r="D12">
+        <v>1.727752591727</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13">
@@ -30499,6 +32660,9 @@
       <c r="C13">
         <v>0.40767251090500001</v>
       </c>
+      <c r="D13">
+        <v>1.8176014621809999</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
@@ -30507,6 +32671,9 @@
       <c r="C14">
         <v>0.41018216037999999</v>
       </c>
+      <c r="D14">
+        <v>1.8139343891619999</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15">
@@ -30515,6 +32682,9 @@
       <c r="C15">
         <v>0.50922963020400003</v>
       </c>
+      <c r="D15">
+        <v>1.7751175792280001</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16">
@@ -30523,196 +32693,341 @@
       <c r="C16">
         <v>0.50845557031599997</v>
       </c>
+      <c r="D16">
+        <v>1.8720210601709999</v>
+      </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>93.088975306747002</v>
       </c>
       <c r="C17">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D17">
+        <v>1.850205428367</v>
+      </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>25.644209351699999</v>
       </c>
       <c r="C18">
         <v>0.406666666668</v>
       </c>
+      <c r="D18">
+        <v>1.886425783357</v>
+      </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>146.686686150822</v>
       </c>
       <c r="C19">
         <v>0.40666666667000001</v>
       </c>
+      <c r="D19">
+        <v>1.873293010841</v>
+      </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>126.28601949976699</v>
       </c>
       <c r="C20">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D20">
+        <v>1.7962052192189999</v>
+      </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>6.8681103691379999</v>
       </c>
+      <c r="D21">
+        <v>1.7248043782810001</v>
+      </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>206.180580524639</v>
       </c>
+      <c r="D22">
+        <v>1.8103600310379999</v>
+      </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>108.935763302745</v>
       </c>
+      <c r="D23">
+        <v>1.9639995861290001</v>
+      </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>0.61000000000200005</v>
       </c>
+      <c r="D24">
+        <v>1.8158170013020001</v>
+      </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>57.004984865182003</v>
       </c>
+      <c r="D25">
+        <v>1.8030894014679999</v>
+      </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0.406666666668</v>
       </c>
+      <c r="D26">
+        <v>1.696682396957</v>
+      </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>81.924129276520006</v>
       </c>
+      <c r="D27">
+        <v>1.7145619581639999</v>
+      </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D28">
+        <v>1.8797401009720001</v>
+      </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>172.58504778538099</v>
       </c>
+      <c r="D29">
+        <v>1.9614644070739999</v>
+      </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>112.22294146845501</v>
       </c>
+      <c r="D30">
+        <v>1.9637167072349999</v>
+      </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>82.493223301520004</v>
       </c>
+      <c r="D31">
+        <v>1.967194162028</v>
+      </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D32">
+        <v>1.764033215385</v>
+      </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>66.505326795643001</v>
       </c>
+      <c r="D33">
+        <v>1.809707220055</v>
+      </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D34">
+        <v>1.858796339907</v>
+      </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>69.807717030917999</v>
       </c>
+      <c r="D35">
+        <v>1.799679362784</v>
+      </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>247.577805762926</v>
       </c>
+      <c r="D36">
+        <v>1.841549727986</v>
+      </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>244.51641065726699</v>
       </c>
+      <c r="D37">
+        <v>1.7612160360269999</v>
+      </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>219.029127908878</v>
       </c>
+      <c r="D38">
+        <v>1.6850714702489999</v>
+      </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>148.981853841163</v>
       </c>
+      <c r="D39">
+        <v>1.7138943863289999</v>
+      </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>0.50833333333499997</v>
       </c>
+      <c r="D40">
+        <v>1.7252054494669999</v>
+      </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>14.368073256500001</v>
       </c>
+      <c r="D41">
+        <v>1.7889433423079999</v>
+      </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>0.61000000000200005</v>
       </c>
+      <c r="D42">
+        <v>1.8763443895680001</v>
+      </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>249.06878495392399</v>
       </c>
+      <c r="D43">
+        <v>1.807917260585</v>
+      </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>1.581761433437</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>1.6580679536139999</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>1.6672101855599999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>1.8559922550700001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>1.969459864124</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>1.7873279270589999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>1.8131713341689999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>1.8999536691900001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>1.6895376699769999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54">
         <v>86.681269999999998</v>
       </c>
-      <c r="C45">
+      <c r="C54">
         <v>0.45000190000000001</v>
       </c>
+      <c r="D54">
+        <v>1.7882979999999999</v>
+      </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55">
         <v>81.924459999999996</v>
       </c>
-      <c r="C46">
+      <c r="C55">
         <v>5.1275830000000001E-2</v>
       </c>
+      <c r="D55">
+        <v>0.1184438</v>
+      </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56">
         <v>16.056899999999999</v>
       </c>
-      <c r="C47">
+      <c r="C56">
         <v>1.0049880000000001E-2</v>
       </c>
+      <c r="D56">
+        <v>2.321455E-2</v>
+      </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57">
         <v>0</v>
       </c>
-      <c r="C48">
+      <c r="C57">
         <v>19</v>
       </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58">
         <v>42</v>
       </c>
-      <c r="C49">
+      <c r="C58">
         <v>0</v>
+      </c>
+      <c r="D58">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30938,15 +33253,15 @@
         <v>0.99547047071648975</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:I30" si="0">(D7-I7)/D7</f>
+        <f>(D7-I7)/D7</f>
         <v>0.99549890752627657</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f>(E7-J7)/E7</f>
         <v>0.99546371771632036</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
+        <f>(F7-K7)/F7</f>
         <v>0.99555695778520559</v>
       </c>
       <c r="J30" s="4">
@@ -30958,15 +33273,15 @@
         <v>0.9778921826281346</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:O30" si="1">(D7-N7)/D7</f>
+        <f>(D7-N7)/D7</f>
         <v>0.97953026428030643</v>
       </c>
       <c r="N30">
-        <f t="shared" si="1"/>
+        <f>(E7-O7)/E7</f>
         <v>0.97834538569162122</v>
       </c>
       <c r="O30">
-        <f t="shared" si="1"/>
+        <f>(F7-P7)/F7</f>
         <v>0.97871374379970455</v>
       </c>
       <c r="P30" s="4">
@@ -31290,11 +33605,11 @@
     </row>
     <row r="30" spans="5:23" x14ac:dyDescent="0.3">
       <c r="H30">
-        <f>(C4-J4)/C4</f>
+        <f t="shared" ref="H30:M30" si="0">(C4-J4)/C4</f>
         <v>0.96150198322408276</v>
       </c>
       <c r="I30">
-        <f t="shared" ref="I30:M30" si="0">(D4-K4)/D4</f>
+        <f t="shared" si="0"/>
         <v>0.95272145230274885</v>
       </c>
       <c r="J30">
@@ -31318,11 +33633,11 @@
         <v>0.98232077183433775</v>
       </c>
       <c r="Q30">
-        <f>(C4-Q4)/C4</f>
+        <f t="shared" ref="Q30:V30" si="1">(C4-Q4)/C4</f>
         <v>1</v>
       </c>
       <c r="R30">
-        <f t="shared" ref="R30:V30" si="1">(D4-R4)/D4</f>
+        <f t="shared" si="1"/>
         <v>0.88413070084420298</v>
       </c>
       <c r="S30">
@@ -31653,19 +33968,19 @@
         <v>0.99986668215009811</v>
       </c>
       <c r="G29">
-        <f t="shared" ref="G29:J29" si="0">(D3-J3)/D3</f>
+        <f>(D3-J3)/D3</f>
         <v>0.99936259558209262</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f>(E3-K3)/E3</f>
         <v>0.99547047071648975</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f>(F3-L3)/F3</f>
         <v>0.98674173582582547</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f>(G3-M3)/G3</f>
         <v>0.99662389032753962</v>
       </c>
       <c r="K29" s="4">
@@ -31677,19 +33992,19 @@
         <v>0.99712565664802633</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:R29" si="1">(D3-P3)/D3</f>
+        <f>(D3-P3)/D3</f>
         <v>0.99463826550543022</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
+        <f>(E3-Q3)/E3</f>
         <v>0.9778921826281346</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
+        <f>(F3-R3)/F3</f>
         <v>0.9475277445629654</v>
       </c>
       <c r="R29">
-        <f t="shared" si="1"/>
+        <f>(G3-S3)/G3</f>
         <v>0.9899236073389972</v>
       </c>
       <c r="S29" s="4">
@@ -32016,11 +34331,11 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E29">
-        <f>(C4-J4)/C4</f>
+        <f t="shared" ref="E29:J29" si="0">(C4-J4)/C4</f>
         <v>0.99547047071648975</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:J29" si="0">(D4-K4)/D4</f>
+        <f t="shared" si="0"/>
         <v>0.99474019809482062</v>
       </c>
       <c r="G29">
@@ -32044,11 +34359,11 @@
         <v>0.99502468531653265</v>
       </c>
       <c r="N29">
-        <f>(C4-Q4)/C4</f>
+        <f t="shared" ref="N29:S29" si="1">(C4-Q4)/C4</f>
         <v>0.9277894283461654</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:S29" si="1">(D4-R4)/D4</f>
+        <f t="shared" si="1"/>
         <v>0.97469217491102256</v>
       </c>
       <c r="P29">
@@ -32084,7 +34399,7 @@
   <dimension ref="A3:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A12:A19"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32345,19 +34660,19 @@
         <v>0.99431821375200202</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:I29" si="0">(C3-I3)/C3</f>
+        <f>(C3-I3)/C3</f>
         <v>0.98628375898129728</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f>(D3-J3)/D3</f>
         <v>0.99707157966450177</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f>(E3-K3)/E3</f>
         <v>0.99976864347927508</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f>(F3-L3)/F3</f>
         <v>0.99997475813701686</v>
       </c>
       <c r="J29" s="4">
@@ -32369,19 +34684,19 @@
         <v>0.98137568641926787</v>
       </c>
       <c r="N29">
-        <f t="shared" ref="N29:Q29" si="1">(C3-O3)/C3</f>
+        <f>(C3-O3)/C3</f>
         <v>0.93820381712013656</v>
       </c>
       <c r="O29">
-        <f t="shared" si="1"/>
+        <f>(D3-P3)/D3</f>
         <v>0.98629391103967168</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
+        <f>(E3-Q3)/E3</f>
         <v>0.99889434571323599</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
+        <f>(F3-R3)/F3</f>
         <v>0.99987866700189032</v>
       </c>
       <c r="R29" s="4">
@@ -32661,19 +34976,19 @@
         <v>0.98587888108630684</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:K29" si="0">(C4-I4)/C4</f>
+        <f>(C4-I4)/C4</f>
         <v>0.98869411023678233</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
+        <f>(D4-J4)/D4</f>
         <v>0.99542963678035956</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f>(E4-K4)/E4</f>
         <v>0.99140906018582842</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
+        <f>(F4-L4)/F4</f>
         <v>0.99556340954833089</v>
       </c>
       <c r="L29" s="4">
@@ -32685,19 +35000,19 @@
         <v>0.95885946849196557</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:R29" si="1">(C4-O4)/C4</f>
+        <f>(C4-O4)/C4</f>
         <v>0.95694562859447285</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
+        <f>(D4-P4)/D4</f>
         <v>0.97510603056271639</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
+        <f>(E4-Q4)/E4</f>
         <v>0.94923834456929845</v>
       </c>
       <c r="R29">
-        <f t="shared" si="1"/>
+        <f>(F4-R4)/F4</f>
         <v>0.98722845641964785</v>
       </c>
       <c r="S29" s="4">

</xml_diff>

<commit_message>
calculated incremental percentuale variation of all experiments
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3E9C17-C08B-421C-BCDF-1414BA1BF7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7811D40-7377-459D-BEBC-9ED9DF87FEC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="Average percentuale variation" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -171,7 +170,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -186,6 +185,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -32121,10 +32123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:Z32"/>
+  <dimension ref="B4:Z36"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="G14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z36" activeCellId="1" sqref="Q36 Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32442,7 +32444,7 @@
     </row>
     <row r="32" spans="4:26" x14ac:dyDescent="0.3">
       <c r="K32">
-        <f t="shared" ref="K32:P32" si="0">(B4-I4)/B4</f>
+        <f t="shared" ref="K32:P34" si="0">(B4-I4)/B4</f>
         <v>0.91152674268280764</v>
       </c>
       <c r="L32">
@@ -32496,6 +32498,68 @@
       <c r="Z32" s="4">
         <f>AVERAGE(T32:Y32)</f>
         <v>0.87734335146299125</v>
+      </c>
+    </row>
+    <row r="33" spans="4:26" x14ac:dyDescent="0.3">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="36" spans="4:26" x14ac:dyDescent="0.3">
+      <c r="J36" s="2"/>
+      <c r="K36" s="2">
+        <f>(B4-I4)/I4</f>
+        <v>10.302850492039886</v>
+      </c>
+      <c r="L36" s="2">
+        <f>(C4-J4)/J4</f>
+        <v>22.712887800585644</v>
+      </c>
+      <c r="M36" s="2">
+        <f>(D4-K4)/K4</f>
+        <v>26.005254749358109</v>
+      </c>
+      <c r="N36" s="2">
+        <f>(E4-L4)/L4</f>
+        <v>69.624008601117083</v>
+      </c>
+      <c r="O36" s="2">
+        <f>(F4-M4)/M4</f>
+        <v>219.773492654189</v>
+      </c>
+      <c r="P36" s="2">
+        <f>(G4-N4)/N4</f>
+        <v>321.68515125108252</v>
+      </c>
+      <c r="Q36" s="10">
+        <f>AVERAGE(K36:P36)</f>
+        <v>111.6839409247287</v>
+      </c>
+      <c r="T36" s="2">
+        <f>(B4-P4)/P4</f>
+        <v>2.0873637428428014</v>
+      </c>
+      <c r="U36" s="2">
+        <f t="shared" ref="U36:Y36" si="2">(C4-Q4)/Q4</f>
+        <v>5.5755633417516046</v>
+      </c>
+      <c r="V36" s="2">
+        <f t="shared" si="2"/>
+        <v>5.3757346687716661</v>
+      </c>
+      <c r="W36" s="2">
+        <f t="shared" si="2"/>
+        <v>14.085554770711473</v>
+      </c>
+      <c r="X36" s="2">
+        <f t="shared" si="2"/>
+        <v>44.23286868076854</v>
+      </c>
+      <c r="Y36" s="2">
+        <f t="shared" si="2"/>
+        <v>66.936327174473718</v>
+      </c>
+      <c r="Z36" s="10">
+        <f>AVERAGE(T36:Y36)</f>
+        <v>23.04890206321997</v>
       </c>
     </row>
   </sheetData>
@@ -32506,10 +32570,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EED80D-1FFC-4B2F-BCEF-819117E61827}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I64" activeCellId="1" sqref="H64 I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32950,27 +33014,27 @@
         <v>1.969459864124</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49">
         <v>1.7873279270589999</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50">
         <v>1.8131713341689999</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D51">
         <v>1.8999536691900001</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>1.6895376699769999</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>86.681269999999998</v>
       </c>
@@ -32981,7 +33045,7 @@
         <v>1.7882979999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>81.924459999999996</v>
       </c>
@@ -32992,7 +33056,7 @@
         <v>0.1184438</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>16.056899999999999</v>
       </c>
@@ -33003,7 +33067,7 @@
         <v>2.321455E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>0</v>
       </c>
@@ -33014,7 +33078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>42</v>
       </c>
@@ -33023,6 +33087,16 @@
       </c>
       <c r="D58">
         <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H64" s="11">
+        <f>(B54-C54)/C54</f>
+        <v>191.62423114213516</v>
+      </c>
+      <c r="I64" s="11">
+        <f>(B54-D54)/D54</f>
+        <v>47.471378931251955</v>
       </c>
     </row>
   </sheetData>
@@ -33033,82 +33107,131 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D7D066-7EAF-4F60-9AB6-0801A04E18F0}">
-  <dimension ref="B3:C11"/>
+  <dimension ref="B3:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>0.96842295594802164</v>
       </c>
       <c r="C4" s="4">
         <v>0.87734335146299125</v>
       </c>
+      <c r="G4" s="10">
+        <v>111.6839409247287</v>
+      </c>
+      <c r="H4" s="10">
+        <v>23.04890206321997</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>0.99549751343607307</v>
       </c>
       <c r="C5" s="4">
         <v>0.97862039409994173</v>
       </c>
+      <c r="G5" s="10">
+        <v>221.11440600810576</v>
+      </c>
+      <c r="H5" s="10">
+        <v>45.810920436814712</v>
+      </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>0.98232077183433775</v>
       </c>
       <c r="C6" s="4">
         <v>0.95796251894277984</v>
       </c>
+      <c r="G6" s="10">
+        <v>140.04109562187443</v>
+      </c>
+      <c r="H6" s="10">
+        <v>34.950992209812767</v>
+      </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>0.99561307492040907</v>
       </c>
       <c r="C7" s="4">
         <v>0.98142149133671075</v>
       </c>
+      <c r="G7" s="10">
+        <v>1931.4261550060626</v>
+      </c>
+      <c r="H7" s="10">
+        <v>138.58895661206944</v>
+      </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>0.99502468531653265</v>
       </c>
       <c r="C8" s="4">
         <v>0.96943795622675299</v>
       </c>
+      <c r="G8" s="10">
+        <v>202.29037827167042</v>
+      </c>
+      <c r="H8" s="10">
+        <v>17.250707378714413</v>
+      </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>0.99548339080281867</v>
       </c>
       <c r="C9" s="4">
         <v>0.98092928545884051</v>
       </c>
+      <c r="G9" s="10">
+        <v>8904.8897656205681</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1856.8117223032809</v>
+      </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>0.99139501956752163</v>
       </c>
       <c r="C10" s="4">
         <v>0.96547558572762016</v>
       </c>
+      <c r="G10" s="10">
+        <v>142.97327896871067</v>
+      </c>
+      <c r="H10" s="10">
+        <v>36.140545317566875</v>
+      </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <f>AVERAGE(B4:B10)</f>
         <v>0.98910820168938773</v>
@@ -33116,6 +33239,22 @@
       <c r="C11" s="5">
         <f>AVERAGE(C4:C10)</f>
         <v>0.95874151189366241</v>
+      </c>
+      <c r="G11" s="11">
+        <v>191.62423114213516</v>
+      </c>
+      <c r="H11" s="11">
+        <v>47.471378931251955</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="12">
+        <f>AVERAGE(G4:G11)</f>
+        <v>1480.7554064454821</v>
+      </c>
+      <c r="H12" s="12">
+        <f>AVERAGE(H4:H11)</f>
+        <v>275.00926565659131</v>
       </c>
     </row>
   </sheetData>
@@ -33125,10 +33264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C216289-8C12-498E-A0E3-71650F3444CE}">
-  <dimension ref="C7:P30"/>
+  <dimension ref="C7:P33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P33" activeCellId="1" sqref="J33 P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33287,6 +33426,48 @@
       <c r="P30" s="4">
         <f>AVERAGE(L30:O30)</f>
         <v>0.97862039409994173</v>
+      </c>
+    </row>
+    <row r="33" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F33" s="2">
+        <f>(C7-H7)/H7</f>
+        <v>219.773492654189</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" ref="G33:I33" si="0">(D7-I7)/I7</f>
+        <v>221.16828599674676</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>219.44483510158915</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>224.0710102798981</v>
+      </c>
+      <c r="J33" s="10">
+        <f>AVERAGE(F33:I33)</f>
+        <v>221.11440600810576</v>
+      </c>
+      <c r="L33" s="2">
+        <f>(C7-M7)/M7</f>
+        <v>44.23286868076854</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" ref="M33:O33" si="1">(D7-N7)/N7</f>
+        <v>47.85260922240041</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="1"/>
+        <v>45.179534105720386</v>
+      </c>
+      <c r="O33" s="2">
+        <f t="shared" si="1"/>
+        <v>45.978669738369518</v>
+      </c>
+      <c r="P33" s="10">
+        <f>AVERAGE(L33:O33)</f>
+        <v>45.810920436814712</v>
       </c>
     </row>
   </sheetData>
@@ -33299,8 +33480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306EBCAD-CACF-4C45-B6AB-C5660DFC9901}">
   <dimension ref="C4:W45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="W32" activeCellId="1" sqref="N32 W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33661,6 +33842,63 @@
         <v>0.95796251894277984</v>
       </c>
     </row>
+    <row r="32" spans="5:23" x14ac:dyDescent="0.3">
+      <c r="H32" s="2">
+        <f>(C4-J4)/J4</f>
+        <v>24.975364025129636</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" ref="I32:M32" si="2">(D4-K4)/K4</f>
+        <v>20.151241920617242</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="2"/>
+        <v>171.10805279950449</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="2"/>
+        <v>237.36049271375649</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="2"/>
+        <v>195.40295907678282</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>191.24846319545591</v>
+      </c>
+      <c r="N32" s="10">
+        <f>AVERAGE(H32:M32)</f>
+        <v>140.04109562187443</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" ref="R32:V32" si="3">(D4-R4)/R4</f>
+        <v>7.6304138135452719</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>37.949006906522186</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="3"/>
+        <v>48.812766168004195</v>
+      </c>
+      <c r="U32" s="2">
+        <f t="shared" si="3"/>
+        <v>40.488759914412697</v>
+      </c>
+      <c r="V32" s="2">
+        <f t="shared" si="3"/>
+        <v>39.874014246579485</v>
+      </c>
+      <c r="W32" s="10">
+        <f>AVERAGE(R32:V32)</f>
+        <v>34.950992209812767</v>
+      </c>
+    </row>
     <row r="40" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P40" s="6" t="s">
         <v>3</v>
@@ -33699,10 +33937,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38478DB4-3557-4910-B8FA-B2B513BB4430}">
-  <dimension ref="C3:S29"/>
+  <dimension ref="C3:S32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="C15:D23"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S31" activeCellId="1" sqref="K31 S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34012,6 +34250,59 @@
         <v>0.98142149133671075</v>
       </c>
     </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="F31" s="2">
+        <f>(C3-I3)/I3</f>
+        <v>7499.8710441690364</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" ref="G31:J31" si="0">(D3-J3)/J3</f>
+        <v>1567.8626747881872</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>219.773492654189</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>74.424654906777107</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="0"/>
+        <v>295.19890851212313</v>
+      </c>
+      <c r="K31" s="10">
+        <f>AVERAGE(F31:J31)</f>
+        <v>1931.4261550060626</v>
+      </c>
+      <c r="N31" s="2">
+        <f>(C3-O3)/O3</f>
+        <v>346.90554834492934</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" ref="O31:R31" si="1">(D3-P3)/P3</f>
+        <v>185.50681062494931</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="1"/>
+        <v>44.23286868076854</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="1"/>
+        <v>18.057690424608783</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="1"/>
+        <v>98.241864985091155</v>
+      </c>
+      <c r="S31" s="10">
+        <f>AVERAGE(N31:R31)</f>
+        <v>138.58895661206944</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="N32" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34020,10 +34311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E897947A-A8E4-4A23-8CE5-CEE211D032C2}">
-  <dimension ref="A4:V29"/>
+  <dimension ref="A4:V31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A14:A20"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T31" activeCellId="1" sqref="K31 T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34387,6 +34678,64 @@
         <v>0.96943795622675299</v>
       </c>
     </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E31" s="2">
+        <f>(C4-J4)/J4</f>
+        <v>219.773492654189</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:J31" si="2">(D4-K4)/K4</f>
+        <v>189.12122852294189</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>181.08790627126245</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="2"/>
+        <v>174.71703297517496</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="2"/>
+        <v>232.59982095878269</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="2"/>
+        <v>216.44278824767164</v>
+      </c>
+      <c r="K31" s="10">
+        <f>AVERAGE(E31:J31)</f>
+        <v>202.29037827167042</v>
+      </c>
+      <c r="N31" s="2">
+        <f>(C4-Q8)/Q4</f>
+        <v>13.848387806619693</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" ref="O31:S31" si="3">(D4-R8)/R4</f>
+        <v>4.6581074124882713</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="3"/>
+        <v>4.5111612351248347</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="3"/>
+        <v>11.251237741000216</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="3"/>
+        <v>31.467514476857687</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>37.767835600195781</v>
+      </c>
+      <c r="T31" s="10">
+        <f>AVERAGE(N31:S31)</f>
+        <v>17.250707378714413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -34396,10 +34745,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8F5EA9-4FF5-47A7-AB2D-15BEFA17A709}">
-  <dimension ref="A3:R29"/>
+  <dimension ref="A3:R31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="R31" activeCellId="1" sqref="J31 R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34704,6 +35053,56 @@
         <v>0.98092928545884051</v>
       </c>
     </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E31" s="2">
+        <f>(B3-H3)/H3</f>
+        <v>175.00098918757209</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:I31" si="0">(C3-I3)/I3</f>
+        <v>71.906272107383771</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>340.48103258196903</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>4321.3333272230675</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>39615.727207002848</v>
+      </c>
+      <c r="J31" s="10">
+        <f>AVERAGE(E31:I31)</f>
+        <v>8904.8897656205681</v>
+      </c>
+      <c r="M31" s="2">
+        <f>(B3-N3)/N3</f>
+        <v>52.693254017939203</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" ref="N31:Q31" si="1">(C3-O3)/O3</f>
+        <v>15.182229280149501</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" si="1"/>
+        <v>71.960273561222124</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="1"/>
+        <v>903.44184223871662</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="1"/>
+        <v>8240.7810124183761</v>
+      </c>
+      <c r="R31" s="10">
+        <f>AVERAGE(M31:Q31)</f>
+        <v>1856.8117223032809</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -34712,10 +35111,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBEEE35-85AF-42CA-8BFA-768200CAE9AB}">
-  <dimension ref="A4:S29"/>
+  <dimension ref="A4:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="A14:B20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S31" activeCellId="1" sqref="L31 S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35018,6 +35417,56 @@
       <c r="S29" s="4">
         <f>AVERAGE(N29:R29)</f>
         <v>0.96547558572762016</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G31" s="2">
+        <f>(B4-H4)/H4</f>
+        <v>69.815918066542139</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" ref="H31:K31" si="0">(C4-I4)/I4</f>
+        <v>87.449473764849643</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>217.80099063082824</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="0"/>
+        <v>115.40170012021447</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="0"/>
+        <v>224.39831226111889</v>
+      </c>
+      <c r="L31" s="10">
+        <f>AVERAGE(G31:K31)</f>
+        <v>142.97327896871067</v>
+      </c>
+      <c r="N31" s="2">
+        <f>(B4-N4)/N4</f>
+        <v>23.306929525320044</v>
+      </c>
+      <c r="O31" s="2">
+        <f t="shared" ref="O31:R31" si="1">(C4-O4)/O4</f>
+        <v>22.226445244805582</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="1"/>
+        <v>39.170371483717851</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="1"/>
+        <v>18.699909144318077</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="1"/>
+        <v>77.29907118967283</v>
+      </c>
+      <c r="S31" s="10">
+        <f>AVERAGE(N31:R31)</f>
+        <v>36.140545317566875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data set clean up
</commit_message>
<xml_diff>
--- a/Data Collections/Combined Data.xlsx
+++ b/Data Collections/Combined Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoga\Desktop\Thesis\TrustChain-Simulator\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79DF983-1125-4126-9A7C-00E99D1B3C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD9D9DC-2A3E-4736-A695-B00D11C9BF7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32331,15 +32331,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:AD36"/>
+  <dimension ref="B3:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>4.5390360000000003</v>
       </c>
@@ -32413,7 +32416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>7.9502920000000001</v>
       </c>
@@ -32487,7 +32490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>1.5582290000000001</v>
       </c>
@@ -32561,7 +32564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>22</v>
       </c>
@@ -32635,7 +32638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>78</v>
       </c>
@@ -32774,27 +32777,27 @@
         <v>0.96842295594802164</v>
       </c>
       <c r="X32">
-        <f>(B4-T4)/B4</f>
+        <f t="shared" ref="X32:AC32" si="1">(B4-T4)/B4</f>
         <v>0.67609906596907365</v>
       </c>
       <c r="Y32">
-        <f>(C4-U4)/C4</f>
+        <f t="shared" si="1"/>
         <v>0.84792177521118384</v>
       </c>
       <c r="Z32">
-        <f>(D4-V4)/D4</f>
+        <f t="shared" si="1"/>
         <v>0.84315533002055465</v>
       </c>
       <c r="AA32">
-        <f>(E4-W4)/E4</f>
+        <f t="shared" si="1"/>
         <v>0.93371142028256759</v>
       </c>
       <c r="AB32">
-        <f>(F4-X4)/F4</f>
+        <f t="shared" si="1"/>
         <v>0.9778921826281346</v>
       </c>
       <c r="AC32">
-        <f>(G4-Y4)/G4</f>
+        <f t="shared" si="1"/>
         <v>0.98528033466643239</v>
       </c>
       <c r="AD32" s="4">
@@ -32808,23 +32811,23 @@
     <row r="36" spans="4:30" x14ac:dyDescent="0.3">
       <c r="L36" s="2"/>
       <c r="M36" s="2">
-        <f t="shared" ref="M36:Q36" si="1">(B4-K4)/K4</f>
+        <f t="shared" ref="M36:Q36" si="2">(B4-K4)/K4</f>
         <v>10.302850492039886</v>
       </c>
       <c r="N36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22.712887800585644</v>
       </c>
       <c r="O36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.005254749358109</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69.624008601117083</v>
       </c>
       <c r="Q36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>219.773492654189</v>
       </c>
       <c r="R36" s="2"/>
@@ -32837,31 +32840,31 @@
         <v>341.96323128345506</v>
       </c>
       <c r="X36" s="2">
-        <f>(B4-T4)/T4</f>
+        <f t="shared" ref="X36:AD36" si="3">(B4-T4)/T4</f>
         <v>2.0873637428428014</v>
       </c>
       <c r="Y36" s="2">
-        <f>(C4-U4)/U4</f>
+        <f t="shared" si="3"/>
         <v>5.5755633417516046</v>
       </c>
       <c r="Z36" s="2">
-        <f>(D4-V4)/V4</f>
+        <f t="shared" si="3"/>
         <v>5.3757346687716661</v>
       </c>
       <c r="AA36" s="2">
-        <f>(E4-W4)/W4</f>
+        <f t="shared" si="3"/>
         <v>14.085554770711473</v>
       </c>
       <c r="AB36" s="2">
-        <f>(F4-X4)/X4</f>
+        <f t="shared" si="3"/>
         <v>44.23286868076854</v>
       </c>
       <c r="AC36" s="2">
-        <f>(G4-Y4)/Y4</f>
+        <f t="shared" si="3"/>
         <v>66.936327174473718</v>
       </c>
       <c r="AD36" s="2">
-        <f>(H4-Z4)/Z4</f>
+        <f t="shared" si="3"/>
         <v>131.33211153228638</v>
       </c>
     </row>

</xml_diff>